<commit_message>
Creación del reporte para la evaluación de desempeño
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
@@ -514,6 +514,123 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -526,80 +643,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -632,84 +710,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1203,11 +1203,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="181614000"/>
-        <c:axId val="181614392"/>
+        <c:axId val="213889960"/>
+        <c:axId val="213890352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181614000"/>
+        <c:axId val="213889960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1217,7 +1217,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181614392"/>
+        <c:crossAx val="213890352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1225,7 +1225,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181614392"/>
+        <c:axId val="213890352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1312,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181614000"/>
+        <c:crossAx val="213889960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1428,7 +1428,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$56</c:f>
+              <c:f>Sheet1!$F$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1440,7 +1440,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$57:$E$64</c:f>
+              <c:f>Sheet1!$E$53:$E$60</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1472,7 +1472,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$57:$F$64</c:f>
+              <c:f>Sheet1!$F$53:$F$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1514,11 +1514,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="204199672"/>
-        <c:axId val="204200064"/>
+        <c:axId val="213891136"/>
+        <c:axId val="213891528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="204199672"/>
+        <c:axId val="213891136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,7 +1528,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204200064"/>
+        <c:crossAx val="213891528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1536,7 +1536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204200064"/>
+        <c:axId val="213891528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1623,7 @@
             <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204199672"/>
+        <c:crossAx val="213891136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2005,10 +2005,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M87"/>
+  <dimension ref="A1:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64:E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,106 +2029,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
       <c r="L2" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="73" t="s">
+      <c r="G4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="74"/>
-      <c r="E6" s="74"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="76" t="s">
+      <c r="G6" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="76"/>
-      <c r="I6" s="74"/>
-      <c r="J6" s="74"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
@@ -2257,327 +2257,339 @@
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="79"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79" t="s">
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="80" t="s">
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="24" t="s">
         <v>34</v>
       </c>
       <c r="L34" s="7"/>
       <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
+      <c r="A35" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="38"/>
-      <c r="C35" s="38"/>
-      <c r="D35" s="38"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="34">
+      <c r="B35" s="36"/>
+      <c r="C35" s="36"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
+      <c r="K35" s="53">
         <v>2</v>
       </c>
       <c r="L35" s="7"/>
       <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="41"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="35"/>
+      <c r="A36" s="38"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="48"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="54"/>
       <c r="L36" s="7"/>
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
-      <c r="B37" s="41"/>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-      <c r="I37" s="29"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="35"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="48"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="54"/>
       <c r="L37" s="7"/>
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="43"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="36"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="43"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="55"/>
       <c r="L38" s="7"/>
       <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="37"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="39"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="22"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="46"/>
+      <c r="K39" s="56"/>
       <c r="L39" s="7"/>
       <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="41"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="23"/>
+      <c r="A40" s="38"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
+      <c r="I40" s="48"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="57"/>
       <c r="L40" s="7"/>
       <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-      <c r="I41" s="29"/>
-      <c r="J41" s="30"/>
-      <c r="K41" s="23"/>
+      <c r="A41" s="38"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="57"/>
       <c r="L41" s="7"/>
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="43"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="24"/>
+      <c r="A42" s="41"/>
+      <c r="B42" s="42"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="58"/>
       <c r="L42" s="7"/>
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="37"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="26"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="22"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="36"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="56"/>
       <c r="L43" s="7"/>
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="B44" s="41"/>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="42"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="23"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="57"/>
       <c r="L44" s="7"/>
       <c r="M44" s="2"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
-      <c r="B45" s="41"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="42"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="29"/>
-      <c r="J45" s="30"/>
-      <c r="K45" s="23"/>
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="57"/>
       <c r="L45" s="7"/>
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="43"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="24"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="42"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="42"/>
+      <c r="E46" s="43"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="51"/>
+      <c r="H46" s="51"/>
+      <c r="I46" s="51"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="58"/>
       <c r="L46" s="7"/>
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="37"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="34"/>
+      <c r="A47" s="71"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="71"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
+      <c r="H47" s="72"/>
+      <c r="I47" s="72"/>
+      <c r="J47" s="72"/>
+      <c r="K47" s="73"/>
       <c r="L47" s="7"/>
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="30"/>
-      <c r="K48" s="35"/>
+      <c r="A48" s="71"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="71"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="72"/>
+      <c r="G48" s="72"/>
+      <c r="H48" s="72"/>
+      <c r="I48" s="72"/>
+      <c r="J48" s="72"/>
+      <c r="K48" s="73"/>
       <c r="L48" s="7"/>
       <c r="M48" s="2"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41"/>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="29"/>
-      <c r="J49" s="30"/>
-      <c r="K49" s="35"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="71"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="72"/>
+      <c r="K49" s="73"/>
       <c r="L49" s="7"/>
       <c r="M49" s="2"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="43"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
-      <c r="I50" s="32"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="36"/>
+      <c r="A50" s="71"/>
+      <c r="B50" s="71"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="71"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="72"/>
+      <c r="G50" s="72"/>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="72"/>
+      <c r="K50" s="73"/>
       <c r="L50" s="7"/>
       <c r="M50" s="2"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="46"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="46"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="48"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="15"/>
       <c r="L51" s="7"/>
       <c r="M51" s="2"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="46"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="46"/>
-      <c r="E52" s="46"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="47"/>
-      <c r="K52" s="48"/>
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="17"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+      <c r="K52" s="15"/>
       <c r="L52" s="7"/>
       <c r="M52" s="2"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="46"/>
-      <c r="B53" s="46"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="46"/>
-      <c r="E53" s="46"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-      <c r="J53" s="47"/>
-      <c r="K53" s="48"/>
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="20">
+        <v>2</v>
+      </c>
+      <c r="G53" s="17"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="15"/>
       <c r="L53" s="7"/>
       <c r="M53" s="2"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
-      <c r="E54" s="46"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="47"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="47"/>
-      <c r="K54" s="48"/>
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="20">
+        <v>4</v>
+      </c>
+      <c r="G54" s="17"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="15"/>
       <c r="L54" s="7"/>
       <c r="M54" s="2"/>
     </row>
@@ -2586,10 +2598,14 @@
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
+      <c r="E55" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="20">
+        <v>4</v>
+      </c>
+      <c r="G55" s="17"/>
+      <c r="H55" s="18"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
@@ -2601,14 +2617,14 @@
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="77" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" s="78" t="s">
-        <v>34</v>
+      <c r="E56" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F56" s="20">
+        <v>3</v>
       </c>
       <c r="G56" s="17"/>
-      <c r="H56" s="16"/>
+      <c r="H56" s="18"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
@@ -2621,10 +2637,10 @@
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
       <c r="E57" s="19" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F57" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G57" s="17"/>
       <c r="H57" s="18"/>
@@ -2640,10 +2656,10 @@
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="19" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F58" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G58" s="17"/>
       <c r="H58" s="18"/>
@@ -2654,252 +2670,232 @@
       <c r="M58" s="2"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
       <c r="E59" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F59" s="20">
+        <v>42</v>
+      </c>
+      <c r="F59" s="21">
         <v>4</v>
       </c>
       <c r="G59" s="17"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="15"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
       <c r="L59" s="7"/>
       <c r="M59" s="2"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
       <c r="E60" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F60" s="20">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="F60" s="21">
+        <v>2</v>
       </c>
       <c r="G60" s="17"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="15"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
       <c r="L60" s="7"/>
       <c r="M60" s="2"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="20">
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+    </row>
+    <row r="62" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B62" s="69"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="69"/>
+      <c r="G62" s="69"/>
+      <c r="H62" s="69"/>
+      <c r="I62" s="69"/>
+      <c r="J62" s="69"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B64" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="32"/>
+      <c r="D64" s="70">
+        <v>3</v>
+      </c>
+      <c r="E64" s="70"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="77" t="s">
+        <v>13</v>
+      </c>
+      <c r="H64" s="78"/>
+      <c r="I64" s="77" t="s">
+        <v>14</v>
+      </c>
+      <c r="J64" s="78"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="32"/>
+      <c r="D65" s="70">
+        <v>2</v>
+      </c>
+      <c r="E65" s="70"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="79" t="s">
+        <v>15</v>
+      </c>
+      <c r="H65" s="80"/>
+      <c r="I65" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="J65" s="62"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="32"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="70"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="H66" s="80"/>
+      <c r="I66" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="J66" s="64"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="32"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="70"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="80"/>
+      <c r="I67" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="J67" s="66"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G68" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="H68" s="60"/>
+      <c r="I68" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="J68" s="68"/>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G69" s="59">
         <v>5</v>
       </c>
-      <c r="G61" s="17"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="2"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F62" s="20">
-        <v>5</v>
-      </c>
-      <c r="G62" s="17"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="7"/>
-      <c r="M62" s="2"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="21">
-        <v>4</v>
-      </c>
-      <c r="G63" s="17"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="2"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="F64" s="21">
-        <v>2</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="6"/>
-      <c r="I64" s="7"/>
-      <c r="J64" s="7"/>
-      <c r="K64" s="7"/>
-      <c r="L64" s="7"/>
-      <c r="M64" s="2"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-    </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="B66" s="60"/>
-      <c r="C66" s="60"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="60"/>
-      <c r="J66" s="60"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B68" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="59"/>
-      <c r="D68" s="61">
-        <v>3</v>
-      </c>
-      <c r="E68" s="61"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="52" t="s">
-        <v>13</v>
-      </c>
-      <c r="H68" s="53"/>
-      <c r="I68" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="J68" s="53"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B69" s="58" t="s">
-        <v>10</v>
-      </c>
-      <c r="C69" s="59"/>
-      <c r="D69" s="61">
-        <v>2</v>
-      </c>
-      <c r="E69" s="61"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="H69" s="55"/>
-      <c r="I69" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="J69" s="63"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B70" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="59"/>
-      <c r="D70" s="61"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="54" t="s">
-        <v>16</v>
-      </c>
-      <c r="H70" s="55"/>
-      <c r="I70" s="64" t="s">
-        <v>22</v>
-      </c>
-      <c r="J70" s="65"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B71" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="61"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="H71" s="55"/>
-      <c r="I71" s="66" t="s">
-        <v>21</v>
-      </c>
-      <c r="J71" s="67"/>
+      <c r="H69" s="60"/>
+      <c r="I69" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69" s="76"/>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4"/>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G72" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="57"/>
-      <c r="I72" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="J72" s="69"/>
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
+      <c r="J72" s="3"/>
+      <c r="K72" s="3"/>
+      <c r="L72" s="3"/>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G73" s="56">
-        <v>5</v>
-      </c>
-      <c r="H73" s="57"/>
-      <c r="I73" s="50" t="s">
-        <v>19</v>
-      </c>
-      <c r="J73" s="51"/>
-    </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
+      <c r="J73" s="3"/>
+      <c r="K73" s="3"/>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
+      <c r="J74" s="3"/>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
+      <c r="J75" s="3"/>
+      <c r="K75" s="3"/>
+      <c r="L75" s="3"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
@@ -2915,130 +2911,91 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-      <c r="B78" s="3"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="4"/>
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="4"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-      <c r="G80" s="3"/>
-      <c r="H80" s="3"/>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
-    </row>
-    <row r="82" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A82" s="4"/>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="49"/>
-      <c r="E84" s="49"/>
-      <c r="F84" s="49"/>
-      <c r="G84" s="49"/>
-      <c r="H84" s="49"/>
-      <c r="I84" s="49"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-      <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-      <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
+      <c r="D80" s="74"/>
+      <c r="E80" s="74"/>
+      <c r="F80" s="74"/>
+      <c r="G80" s="74"/>
+      <c r="H80" s="74"/>
+      <c r="I80" s="74"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="58">
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
+  <mergeCells count="55">
+    <mergeCell ref="K43:K46"/>
+    <mergeCell ref="F47:J50"/>
+    <mergeCell ref="K47:K50"/>
+    <mergeCell ref="A43:E46"/>
+    <mergeCell ref="A47:E50"/>
+    <mergeCell ref="F43:J46"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="F80:G80"/>
+    <mergeCell ref="H80:I80"/>
+    <mergeCell ref="I69:J69"/>
+    <mergeCell ref="G64:H64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="I64:J64"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="I66:J66"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="I68:J68"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G4:H4"/>
@@ -3052,38 +3009,18 @@
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="G73:H73"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="I70:J70"/>
-    <mergeCell ref="I71:J71"/>
-    <mergeCell ref="I72:J72"/>
     <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A66:J66"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="A51:E54"/>
-    <mergeCell ref="F51:J54"/>
-    <mergeCell ref="K51:K54"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="F84:G84"/>
-    <mergeCell ref="H84:I84"/>
-    <mergeCell ref="I73:J73"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="G70:H70"/>
-    <mergeCell ref="G71:H71"/>
-    <mergeCell ref="G72:H72"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="K43:K46"/>
-    <mergeCell ref="F47:J50"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="A43:E46"/>
-    <mergeCell ref="A47:E50"/>
-    <mergeCell ref="F43:J46"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega la logica dle reporte ED con Nivel de Talento
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,16 +165,13 @@
     <t>Fecha de Registro de Compromisos:</t>
   </si>
   <si>
-    <t>Impreso:</t>
+    <t>Comentarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -269,8 +266,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color theme="1"/>
+      <sz val="8"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,7 +323,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -510,19 +507,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -583,32 +621,157 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -616,73 +779,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -695,93 +801,80 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1239,11 +1332,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="81220352"/>
-        <c:axId val="81221888"/>
+        <c:axId val="91136384"/>
+        <c:axId val="91137920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81220352"/>
+        <c:axId val="91136384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,14 +1345,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="81221888"/>
+        <c:crossAx val="91137920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81221888"/>
+        <c:axId val="91137920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,7 +1436,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81220352"/>
+        <c:crossAx val="91136384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1523,11 +1616,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="81246848"/>
-        <c:axId val="81396096"/>
+        <c:axId val="91957504"/>
+        <c:axId val="91971584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81246848"/>
+        <c:axId val="91957504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,14 +1629,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="81396096"/>
+        <c:crossAx val="91971584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81396096"/>
+        <c:axId val="91971584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1627,7 +1720,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81246848"/>
+        <c:crossAx val="91957504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1673,6 +1766,897 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-ES"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CR"/>
+              <a:t>Nivel de Talento</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$66</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:delete val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$70:$P$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$71:$P$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="0"/>
+        <c:axId val="93406336"/>
+        <c:axId val="93407872"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="93406336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="93407872"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="93407872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="93406336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1736,6 +2720,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1114425</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2008,10 +3022,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:P102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2032,981 +3046,1277 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="10"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="71"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="42" t="s">
+      <c r="C5" s="71"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="42"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="45"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="92"/>
+      <c r="J7" s="92"/>
     </row>
     <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
+      <c r="B9" s="93"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="93"/>
+      <c r="J9" s="93"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="K11" s="11"/>
-      <c r="L11" s="11">
+      <c r="K11" s="10"/>
+      <c r="L11" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="K12" s="11"/>
-      <c r="L12" s="11">
+      <c r="K12" s="10"/>
+      <c r="L12" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="K13" s="11"/>
-      <c r="L13" s="11">
+      <c r="K13" s="10"/>
+      <c r="L13" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="K14" s="11"/>
-      <c r="L14" s="11">
+      <c r="K14" s="10"/>
+      <c r="L14" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
     </row>
     <row r="17" spans="1:13">
-      <c r="K17" s="11" t="s">
+      <c r="K17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="10">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="K19" s="11" t="s">
+      <c r="K19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="10">
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="K20" s="11" t="s">
+      <c r="K20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="11">
+      <c r="L20" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L21" s="11">
+      <c r="L21" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L23" s="11">
+      <c r="L23" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="K24" s="11" t="s">
+      <c r="K24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47" t="s">
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="22" t="s">
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L34" s="7"/>
+      <c r="L34" s="6"/>
       <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1">
-      <c r="A35" s="48" t="s">
+      <c r="A35" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="49"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="57">
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="78">
         <v>2</v>
       </c>
-      <c r="L35" s="7"/>
+      <c r="L35" s="6"/>
       <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="52"/>
-      <c r="D36" s="52"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="53"/>
-      <c r="K36" s="58"/>
-      <c r="L36" s="7"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="6"/>
       <c r="M36" s="2"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="53"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="7"/>
+      <c r="A37" s="39"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="6"/>
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A38" s="54"/>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="55"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="55"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="7"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="43"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="80"/>
+      <c r="L38" s="6"/>
       <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="60"/>
-      <c r="B39" s="61"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="62"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="50"/>
-      <c r="K39" s="69"/>
-      <c r="L39" s="7"/>
+      <c r="A39" s="81"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="48"/>
+      <c r="K39" s="31"/>
+      <c r="L39" s="6"/>
       <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="63"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="64"/>
-      <c r="E40" s="65"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="70"/>
-      <c r="L40" s="7"/>
+      <c r="A40" s="84"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="49"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="I40" s="50"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="6"/>
       <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="64"/>
-      <c r="E41" s="65"/>
-      <c r="F41" s="51"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="53"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="7"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="85"/>
+      <c r="D41" s="85"/>
+      <c r="E41" s="86"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="50"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="50"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="6"/>
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A42" s="66"/>
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="68"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="55"/>
-      <c r="H42" s="55"/>
-      <c r="I42" s="55"/>
-      <c r="J42" s="56"/>
-      <c r="K42" s="71"/>
-      <c r="L42" s="7"/>
+      <c r="A42" s="87"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="89"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="6"/>
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="48"/>
-      <c r="B43" s="49"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="69"/>
-      <c r="L43" s="7"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="37"/>
+      <c r="D43" s="37"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="31"/>
+      <c r="L43" s="6"/>
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="51"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="70"/>
-      <c r="L44" s="7"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="6"/>
       <c r="M44" s="2"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="51"/>
-      <c r="B45" s="52"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="53"/>
-      <c r="K45" s="70"/>
-      <c r="L45" s="7"/>
+      <c r="A45" s="39"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="51"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="6"/>
       <c r="M45" s="2"/>
     </row>
     <row r="46" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A46" s="54"/>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="56"/>
-      <c r="K46" s="71"/>
-      <c r="L46" s="7"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="53"/>
+      <c r="H46" s="53"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="54"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="6"/>
       <c r="M46" s="2"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="48"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="50"/>
-      <c r="K47" s="86"/>
-      <c r="L47" s="7"/>
+      <c r="A47" s="45"/>
+      <c r="B47" s="45"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="35"/>
+      <c r="L47" s="6"/>
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13">
-      <c r="A48" s="51"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="53"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="53"/>
-      <c r="K48" s="86"/>
-      <c r="L48" s="7"/>
+      <c r="A48" s="45"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="6"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:13">
-      <c r="A49" s="51"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="52"/>
-      <c r="H49" s="52"/>
-      <c r="I49" s="52"/>
-      <c r="J49" s="53"/>
-      <c r="K49" s="86"/>
-      <c r="L49" s="7"/>
+    <row r="49" spans="1:16">
+      <c r="A49" s="45"/>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="6"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:13" ht="26.25" customHeight="1">
-      <c r="A50" s="54"/>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
-      <c r="J50" s="56"/>
-      <c r="K50" s="86"/>
-      <c r="L50" s="7"/>
+    <row r="50" spans="1:16" ht="26.25" customHeight="1">
+      <c r="A50" s="45"/>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="35"/>
+      <c r="L50" s="6"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:13">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="7"/>
+    <row r="51" spans="1:16">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="6"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:13">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="26" t="s">
+    <row r="52" spans="1:16">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="25" t="s">
+      <c r="F52" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="7"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="14"/>
+      <c r="L52" s="6"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:13" ht="37.5" customHeight="1">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="19" t="s">
+    <row r="53" spans="1:16" ht="37.5" customHeight="1">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="F53" s="20">
+      <c r="F53" s="19">
         <v>2</v>
       </c>
-      <c r="G53" s="17"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="7"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="6"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="19" t="s">
+    <row r="54" spans="1:16">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="F54" s="20">
+      <c r="F54" s="19">
         <v>4</v>
       </c>
-      <c r="G54" s="17"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="7"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="6"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:13">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="19" t="s">
+    <row r="55" spans="1:16">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F55" s="20">
+      <c r="F55" s="19">
         <v>4</v>
       </c>
-      <c r="G55" s="17"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="7"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="6"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="19" t="s">
+    <row r="56" spans="1:16" ht="18.75" customHeight="1">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="19">
         <v>3</v>
       </c>
-      <c r="G56" s="17"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="7"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="14"/>
+      <c r="L56" s="6"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="19" t="s">
+    <row r="57" spans="1:16" ht="16.5" customHeight="1">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F57" s="20">
+      <c r="F57" s="19">
         <v>5</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="7"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="6"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:13">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="19" t="s">
+    <row r="58" spans="1:16">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F58" s="20">
+      <c r="F58" s="19">
         <v>5</v>
       </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="7"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="14"/>
+      <c r="L58" s="6"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:13">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="12"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="19" t="s">
+    <row r="59" spans="1:16">
+      <c r="A59" s="11"/>
+      <c r="B59" s="11"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F59" s="21">
+      <c r="F59" s="20">
         <v>4</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="19" t="s">
+    <row r="60" spans="1:16">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="21">
+      <c r="F60" s="20">
         <v>2</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+      <c r="K60" s="6"/>
+      <c r="L60" s="6"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:13">
-      <c r="G61" s="5"/>
+    <row r="61" spans="1:16">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="16"/>
       <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-    </row>
-    <row r="62" spans="1:13" ht="15.75">
-      <c r="A62" s="33" t="s">
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="2"/>
+    </row>
+    <row r="62" spans="1:16">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="26"/>
+      <c r="F62" s="27"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="2"/>
+    </row>
+    <row r="63" spans="1:16">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="26"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="2"/>
+    </row>
+    <row r="64" spans="1:16">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="26"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="2"/>
+      <c r="N64" s="29">
+        <v>5</v>
+      </c>
+      <c r="O64" s="30"/>
+      <c r="P64" s="30"/>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="2"/>
+      <c r="N65" s="29">
+        <v>4</v>
+      </c>
+      <c r="O65" s="30"/>
+      <c r="P65" s="30"/>
+    </row>
+    <row r="66" spans="1:16">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="26"/>
+      <c r="F66" s="27"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="2"/>
+      <c r="N66" s="29">
+        <v>3</v>
+      </c>
+      <c r="O66" s="30"/>
+      <c r="P66" s="30"/>
+    </row>
+    <row r="67" spans="1:16">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="2"/>
+      <c r="N67" s="29">
+        <v>2</v>
+      </c>
+      <c r="O67" s="30"/>
+      <c r="P67" s="30"/>
+    </row>
+    <row r="68" spans="1:16">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="29">
+        <v>1</v>
+      </c>
+      <c r="O68" s="30"/>
+      <c r="P68" s="30"/>
+    </row>
+    <row r="69" spans="1:16">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+      <c r="K69" s="6"/>
+      <c r="L69" s="6"/>
+      <c r="M69" s="2"/>
+      <c r="N69" s="29">
+        <v>0</v>
+      </c>
+      <c r="O69" s="30"/>
+      <c r="P69" s="30"/>
+    </row>
+    <row r="70" spans="1:16">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+      <c r="K70" s="6"/>
+      <c r="L70" s="6"/>
+      <c r="M70" s="2"/>
+      <c r="N70" s="29"/>
+      <c r="O70" s="30">
+        <v>2</v>
+      </c>
+      <c r="P70" s="30"/>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
+      <c r="L71" s="6"/>
+      <c r="M71" s="2"/>
+      <c r="N71" s="29"/>
+      <c r="O71" s="30"/>
+      <c r="P71" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="26"/>
+      <c r="F72" s="27"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+      <c r="K72" s="6"/>
+      <c r="L72" s="6"/>
+      <c r="M72" s="2"/>
+    </row>
+    <row r="73" spans="1:16">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+      <c r="K73" s="6"/>
+      <c r="L73" s="6"/>
+      <c r="M73" s="2"/>
+    </row>
+    <row r="74" spans="1:16">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="26"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+      <c r="K74" s="6"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="75" spans="1:16">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="27"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+      <c r="K75" s="6"/>
+      <c r="L75" s="6"/>
+      <c r="M75" s="2"/>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="26"/>
+      <c r="F76" s="27"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="2"/>
+    </row>
+    <row r="77" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A77" s="7"/>
+      <c r="B77" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" s="28"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="26"/>
+      <c r="F77" s="27"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="2"/>
+    </row>
+    <row r="78" spans="1:16">
+      <c r="A78" s="7"/>
+      <c r="B78" s="98"/>
+      <c r="C78" s="99"/>
+      <c r="D78" s="99"/>
+      <c r="E78" s="99"/>
+      <c r="F78" s="99"/>
+      <c r="G78" s="99"/>
+      <c r="H78" s="99"/>
+      <c r="I78" s="99"/>
+      <c r="J78" s="100"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="2"/>
+    </row>
+    <row r="79" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A79" s="7"/>
+      <c r="B79" s="101"/>
+      <c r="C79" s="102"/>
+      <c r="D79" s="102"/>
+      <c r="E79" s="102"/>
+      <c r="F79" s="102"/>
+      <c r="G79" s="102"/>
+      <c r="H79" s="102"/>
+      <c r="I79" s="102"/>
+      <c r="J79" s="103"/>
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="2"/>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="27"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" ht="15.75">
+      <c r="A81" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-    </row>
-    <row r="63" spans="1:13">
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-    </row>
-    <row r="64" spans="1:13">
-      <c r="B64" s="36" t="s">
+      <c r="B81" s="93"/>
+      <c r="C81" s="93"/>
+      <c r="D81" s="93"/>
+      <c r="E81" s="93"/>
+      <c r="F81" s="93"/>
+      <c r="G81" s="93"/>
+      <c r="H81" s="93"/>
+      <c r="I81" s="93"/>
+      <c r="J81" s="93"/>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="B83" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="35">
+      <c r="C83" s="74"/>
+      <c r="D83" s="64">
+        <v>2</v>
+      </c>
+      <c r="E83" s="64"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="59"/>
+      <c r="I83" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="J83" s="59"/>
+    </row>
+    <row r="84" spans="1:12">
+      <c r="B84" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" s="74"/>
+      <c r="D84" s="64">
         <v>3</v>
       </c>
-      <c r="E64" s="35"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="75" t="s">
-        <v>12</v>
-      </c>
-      <c r="H64" s="76"/>
-      <c r="I64" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="J64" s="76"/>
-    </row>
-    <row r="65" spans="1:12">
-      <c r="B65" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" s="37"/>
-      <c r="D65" s="35">
-        <v>2</v>
-      </c>
-      <c r="E65" s="35"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="77" t="s">
+      <c r="E84" s="64"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="78"/>
-      <c r="I65" s="38" t="s">
+      <c r="H84" s="61"/>
+      <c r="I84" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="J65" s="39"/>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="B66" s="36" t="s">
+      <c r="J84" s="95"/>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="B85" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="77" t="s">
+      <c r="C85" s="74"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="H66" s="78"/>
-      <c r="I66" s="40" t="s">
+      <c r="H85" s="61"/>
+      <c r="I85" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="J66" s="41"/>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="B67" s="36" t="s">
+      <c r="J85" s="97"/>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="B86" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="77" t="s">
+      <c r="C86" s="74"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H67" s="78"/>
-      <c r="I67" s="81" t="s">
+      <c r="H86" s="61"/>
+      <c r="I86" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="J67" s="82"/>
-    </row>
-    <row r="68" spans="1:12">
-      <c r="G68" s="79" t="s">
+      <c r="J86" s="66"/>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="G87" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="H68" s="80"/>
-      <c r="I68" s="83" t="s">
+      <c r="H87" s="63"/>
+      <c r="I87" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="J68" s="84"/>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="G69" s="79">
+      <c r="J87" s="68"/>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="G88" s="62">
         <v>5</v>
       </c>
-      <c r="H69" s="80"/>
-      <c r="I69" s="73" t="s">
+      <c r="H88" s="63"/>
+      <c r="I88" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="J69" s="74"/>
-    </row>
-    <row r="73" spans="1:12" ht="15.75">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
-    </row>
-    <row r="75" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A75" s="3"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="23"/>
-      <c r="E75" s="23"/>
-      <c r="F75" s="3"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="85"/>
-      <c r="I75" s="85"/>
-      <c r="J75" s="85"/>
-      <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="3"/>
-      <c r="B76" s="30" t="s">
+      <c r="J88" s="57"/>
+    </row>
+    <row r="92" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A92" s="3"/>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="3"/>
+      <c r="G92" s="3"/>
+      <c r="H92" s="69"/>
+      <c r="I92" s="69"/>
+      <c r="J92" s="69"/>
+      <c r="K92" s="3"/>
+      <c r="L92" s="3"/>
+    </row>
+    <row r="93" spans="1:12">
+      <c r="A93" s="3"/>
+      <c r="B93" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="C76" s="30"/>
-      <c r="D76" s="30"/>
-      <c r="E76" s="30"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="30" t="s">
+      <c r="C93" s="70"/>
+      <c r="D93" s="70"/>
+      <c r="E93" s="70"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="I76" s="30"/>
-      <c r="J76" s="30"/>
-      <c r="K76" s="24"/>
-      <c r="L76" s="24"/>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B78" s="28">
-        <f ca="1">NOW()</f>
-        <v>41887.896211921296</v>
-      </c>
-      <c r="C78" s="29">
-        <f ca="1">NOW()</f>
-        <v>41887.896211921296</v>
-      </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="80" spans="1:12" ht="15.75">
-      <c r="A80" s="4"/>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-    </row>
-    <row r="82" spans="2:9">
-      <c r="B82" s="3"/>
-      <c r="C82" s="3"/>
-      <c r="D82" s="72"/>
-      <c r="E82" s="72"/>
-      <c r="F82" s="72"/>
-      <c r="G82" s="72"/>
-      <c r="H82" s="72"/>
-      <c r="I82" s="72"/>
-    </row>
-    <row r="83" spans="2:9">
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="2:9">
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="2:9">
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
+      <c r="I93" s="70"/>
+      <c r="J93" s="70"/>
+      <c r="K93" s="23"/>
+      <c r="L93" s="23"/>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="A94" s="3"/>
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3"/>
+      <c r="L94" s="3"/>
+    </row>
+    <row r="95" spans="1:12">
+      <c r="A95" s="3"/>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="3"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="3"/>
+      <c r="H95" s="3"/>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3"/>
+      <c r="L95" s="3"/>
+    </row>
+    <row r="97" spans="1:10" ht="15.75">
+      <c r="A97" s="4"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4"/>
+    </row>
+    <row r="99" spans="1:10">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="55"/>
+      <c r="E99" s="55"/>
+      <c r="F99" s="55"/>
+      <c r="G99" s="55"/>
+      <c r="H99" s="55"/>
+      <c r="I99" s="55"/>
+    </row>
+    <row r="100" spans="1:10">
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+      <c r="G100" s="3"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
+    </row>
+    <row r="101" spans="1:10">
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="1:10">
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="58">
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="K43:K46"/>
-    <mergeCell ref="F47:J50"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="A43:E46"/>
-    <mergeCell ref="A47:E50"/>
-    <mergeCell ref="F43:J46"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="I69:J69"/>
-    <mergeCell ref="G64:H64"/>
-    <mergeCell ref="G65:H65"/>
-    <mergeCell ref="G66:H66"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="I64:J64"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="G69:H69"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="I68:J68"/>
-    <mergeCell ref="H75:J75"/>
-    <mergeCell ref="H76:J76"/>
+  <mergeCells count="59">
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="I84:J84"/>
+    <mergeCell ref="I85:J85"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B78:J79"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B86:C86"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G4:H4"/>
@@ -3019,26 +4329,29 @@
     <mergeCell ref="K39:K42"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="I65:J65"/>
-    <mergeCell ref="I66:J66"/>
-    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="F99:G99"/>
+    <mergeCell ref="H99:I99"/>
+    <mergeCell ref="I88:J88"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="G85:H85"/>
+    <mergeCell ref="G86:H86"/>
+    <mergeCell ref="G87:H87"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="G88:H88"/>
+    <mergeCell ref="I86:J86"/>
+    <mergeCell ref="I87:J87"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="K43:K46"/>
+    <mergeCell ref="F47:J50"/>
+    <mergeCell ref="K47:K50"/>
+    <mergeCell ref="A43:E46"/>
+    <mergeCell ref="A47:E50"/>
+    <mergeCell ref="F43:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Modificación de reporte para aceptar 5 puntualizaciones
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Desktop\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Módulo de Evaluación de Desempeño</t>
   </si>
@@ -45,134 +50,140 @@
     <t>Resultados</t>
   </si>
   <si>
+    <t>EVALUACIÓN FINAL</t>
+  </si>
+  <si>
+    <t>RANGO</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Interpretación</t>
+  </si>
+  <si>
+    <t>De 0 a 2</t>
+  </si>
+  <si>
+    <t>Más de 2 menos de 3</t>
+  </si>
+  <si>
+    <t>De 3 a menos de 4</t>
+  </si>
+  <si>
+    <t>De 4 a menos de 5</t>
+  </si>
+  <si>
+    <t>Desempeño Superior</t>
+  </si>
+  <si>
+    <t>Desempeño Sobresaliente</t>
+  </si>
+  <si>
+    <t>Desempeño Esperado</t>
+  </si>
+  <si>
+    <t>Oportunidad de Mejora</t>
+  </si>
+  <si>
+    <t>Desempeño Insuficiente</t>
+  </si>
+  <si>
+    <t>solucion</t>
+  </si>
+  <si>
+    <t>negociacion</t>
+  </si>
+  <si>
+    <t>planificacion</t>
+  </si>
+  <si>
+    <t>trabajar bajo presion</t>
+  </si>
+  <si>
+    <t>tomar decisiones</t>
+  </si>
+  <si>
+    <t>admnistrar tiempo</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>ade</t>
+  </si>
+  <si>
+    <t>Indicador</t>
+  </si>
+  <si>
+    <t>Compromiso</t>
+  </si>
+  <si>
+    <t>Puntaje</t>
+  </si>
+  <si>
+    <t>Cumpliendo con el plan estratégico de la Universidad, aplica los procedimientos que corresponden a la ejecución de las pruebas y todo lo que conlleva (coordinación de matrícula, coordinación de aulas, oidores, jurados, entre otros) interactúa con los clientes internos (compañeros de trabajo) y externos (estudiantes, Jurados y oidores), velar por la correcta aplicación de la Ordenanza y las buenas relaciones con las Sedes, con el fin de planificar y ejecutar el calendario Universitario de las Pruebas de Grado y toda la logística en tiempo establecido.</t>
+  </si>
+  <si>
+    <t>Competencia</t>
+  </si>
+  <si>
+    <t>investigacion</t>
+  </si>
+  <si>
+    <t>logro</t>
+  </si>
+  <si>
+    <t>orientacion</t>
+  </si>
+  <si>
+    <t>esfuerzo</t>
+  </si>
+  <si>
+    <t>Firma Evaluador</t>
+  </si>
+  <si>
+    <t>Firma Colaborador</t>
+  </si>
+  <si>
+    <t>Alineamiento organizacional</t>
+  </si>
+  <si>
+    <t>Pensamiento estrategico</t>
+  </si>
+  <si>
+    <t>Toma de decisiones</t>
+  </si>
+  <si>
+    <t>Fecha de Registro de Evaluación:</t>
+  </si>
+  <si>
+    <t>Fecha de Registro de Compromisos:</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Escala</t>
+  </si>
+  <si>
     <t>Nivel Puntualizaciones</t>
   </si>
   <si>
     <t>Nivel Competencias</t>
   </si>
   <si>
-    <t>EVALUACIÓN FINAL</t>
-  </si>
-  <si>
-    <t>RANGO</t>
-  </si>
-  <si>
-    <t>Rango</t>
-  </si>
-  <si>
-    <t>Interpretación</t>
-  </si>
-  <si>
-    <t>De 0 a 2</t>
-  </si>
-  <si>
-    <t>Más de 2 menos de 3</t>
-  </si>
-  <si>
-    <t>De 3 a menos de 4</t>
-  </si>
-  <si>
-    <t>De 4 a menos de 5</t>
-  </si>
-  <si>
-    <t>Desempeño Superior</t>
-  </si>
-  <si>
-    <t>Desempeño Sobresaliente</t>
-  </si>
-  <si>
-    <t>Desempeño Esperado</t>
-  </si>
-  <si>
-    <t>Oportunidad de Mejora</t>
-  </si>
-  <si>
-    <t>Desempeño Insuficiente</t>
-  </si>
-  <si>
-    <t>solucion</t>
-  </si>
-  <si>
-    <t>negociacion</t>
-  </si>
-  <si>
-    <t>planificacion</t>
-  </si>
-  <si>
-    <t>trabajar bajo presion</t>
-  </si>
-  <si>
-    <t>tomar decisiones</t>
-  </si>
-  <si>
-    <t>admnistrar tiempo</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>ade</t>
-  </si>
-  <si>
-    <t>Indicador</t>
-  </si>
-  <si>
-    <t>Compromiso</t>
-  </si>
-  <si>
-    <t>Puntaje</t>
-  </si>
-  <si>
-    <t>Cumpliendo con el plan estratégico de la Universidad, aplica los procedimientos que corresponden a la ejecución de las pruebas y todo lo que conlleva (coordinación de matrícula, coordinación de aulas, oidores, jurados, entre otros) interactúa con los clientes internos (compañeros de trabajo) y externos (estudiantes, Jurados y oidores), velar por la correcta aplicación de la Ordenanza y las buenas relaciones con las Sedes, con el fin de planificar y ejecutar el calendario Universitario de las Pruebas de Grado y toda la logística en tiempo establecido.</t>
-  </si>
-  <si>
-    <t>Competencia</t>
-  </si>
-  <si>
-    <t>investigacion</t>
-  </si>
-  <si>
-    <t>logro</t>
-  </si>
-  <si>
-    <t>orientacion</t>
-  </si>
-  <si>
-    <t>esfuerzo</t>
-  </si>
-  <si>
-    <t>kkel</t>
-  </si>
-  <si>
-    <t>Firma Evaluador</t>
-  </si>
-  <si>
-    <t>Firma Colaborador</t>
-  </si>
-  <si>
-    <t>Alineamiento organizacional</t>
-  </si>
-  <si>
-    <t>Pensamiento estrategico</t>
-  </si>
-  <si>
-    <t>Toma de decisiones</t>
-  </si>
-  <si>
-    <t>Fecha de Registro de Evaluación:</t>
-  </si>
-  <si>
-    <t>Fecha de Registro de Compromisos:</t>
-  </si>
-  <si>
-    <t>Comentarios</t>
+    <t>trabajo</t>
+  </si>
+  <si>
+    <t>equipo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -633,6 +644,28 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -645,13 +678,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -853,27 +879,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -895,7 +921,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -929,6 +965,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -937,6 +974,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -946,6 +984,7 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -973,6 +1012,7 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -997,6 +1037,7 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1021,6 +1062,7 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1045,6 +1087,7 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1069,6 +1112,7 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1093,6 +1137,7 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1117,6 +1162,7 @@
         <c:ser>
           <c:idx val="7"/>
           <c:order val="7"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1141,6 +1187,7 @@
         <c:ser>
           <c:idx val="8"/>
           <c:order val="8"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1165,6 +1212,7 @@
         <c:ser>
           <c:idx val="9"/>
           <c:order val="9"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1189,6 +1237,7 @@
         <c:ser>
           <c:idx val="10"/>
           <c:order val="10"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1213,6 +1262,7 @@
         <c:ser>
           <c:idx val="11"/>
           <c:order val="11"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1237,6 +1287,7 @@
         <c:ser>
           <c:idx val="12"/>
           <c:order val="12"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1261,6 +1312,7 @@
         <c:ser>
           <c:idx val="13"/>
           <c:order val="13"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1285,6 +1337,7 @@
         <c:ser>
           <c:idx val="14"/>
           <c:order val="14"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1309,6 +1362,7 @@
         <c:ser>
           <c:idx val="15"/>
           <c:order val="15"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1330,13 +1384,121 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="91136384"/>
-        <c:axId val="91137920"/>
+        <c:axId val="182558584"/>
+        <c:axId val="182558976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91136384"/>
+        <c:axId val="182558584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,18 +1506,21 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="91137920"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="182558976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91137920"/>
+        <c:axId val="182558976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1398,6 +1563,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1408,6 +1574,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1433,10 +1600,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91136384"/>
+        <c:crossAx val="182558584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1450,6 +1617,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1473,12 +1641,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1486,7 +1654,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1520,6 +1698,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1528,6 +1707,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1539,7 +1719,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$52</c:f>
+              <c:f>Sheet1!$F$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1548,11 +1728,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$53:$E$60</c:f>
+              <c:f>Sheet1!$E$62:$E$70</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Alineamiento organizacional</c:v>
                 </c:pt>
@@ -1575,17 +1756,20 @@
                   <c:v>esfuerzo</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>kkel</c:v>
+                  <c:v>trabajo</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>equipo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$53:$F$60</c:f>
+              <c:f>Sheet1!$F$62:$F$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1609,18 +1793,29 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="91957504"/>
-        <c:axId val="91971584"/>
+        <c:axId val="182559760"/>
+        <c:axId val="182560152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91957504"/>
+        <c:axId val="182559760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,18 +1823,21 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="91971584"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="182560152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91971584"/>
+        <c:axId val="182560152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1682,6 +1880,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1692,6 +1891,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1717,10 +1917,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91957504"/>
+        <c:crossAx val="182559760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1734,6 +1934,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1757,12 +1958,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1770,7 +1971,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1799,6 +2010,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1806,12 +2018,34 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1826,9 +2060,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$64</c:f>
+              <c:f>Sheet1!$N$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1851,9 +2103,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$65</c:f>
+              <c:f>Sheet1!$N$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1876,9 +2146,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$66</c:f>
+              <c:f>Sheet1!$N$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1901,9 +2189,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$67</c:f>
+              <c:f>Sheet1!$N$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1926,9 +2232,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$68</c:f>
+              <c:f>Sheet1!$N$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1951,9 +2275,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$69</c:f>
+              <c:f>Sheet1!$N$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1976,16 +2318,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:delete val="1"/>
-            </c:dLbl>
-            <c:showVal val="1"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$70:$P$70</c:f>
+              <c:f>Sheet1!$N$80:$P$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2010,9 +2363,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$71:$P$71</c:f>
+              <c:f>Sheet1!$N$81:$P$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2023,32 +2394,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="93406336"/>
-        <c:axId val="93407872"/>
+        <c:axId val="183498408"/>
+        <c:axId val="183498800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93406336"/>
+        <c:axId val="183498408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="93407872"/>
-        <c:crosses val="autoZero"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="93407872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2074,10 +2441,55 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93406336"/>
+        <c:crossAx val="183498800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="183498800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="183498408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2091,6 +2503,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2114,12 +2527,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2729,13 +3142,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2801,7 +3214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2836,7 +3249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3013,22 +3426,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94:E94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -3045,207 +3458,207 @@
     <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="71" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="71" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="B6" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="94"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
+      <c r="G6" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="93" t="s">
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K11" s="10"/>
       <c r="L11" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K12" s="10"/>
       <c r="L12" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K13" s="10"/>
       <c r="L13" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K14" s="10"/>
       <c r="L14" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K17" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L18" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L19" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L20" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K21" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L21" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L24" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -3259,7 +3672,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -3273,589 +3686,565 @@
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="77" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="78">
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="82">
         <v>2</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="39"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="79"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="83"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="39"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="79"/>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="83"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A38" s="42"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="80"/>
+    <row r="38" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="84"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="81"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="31"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="85"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="37"/>
       <c r="L39" s="6"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="84"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="32"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="88"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="38"/>
       <c r="L40" s="6"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="84"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="32"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="88"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="38"/>
       <c r="L41" s="6"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A42" s="87"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="33"/>
+    <row r="42" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="91"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="6"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="31"/>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="40"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="37"/>
       <c r="L43" s="6"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="32"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="43"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="38"/>
       <c r="L44" s="6"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="39"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="32"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="43"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="38"/>
       <c r="L45" s="6"/>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="33"/>
+    <row r="46" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="46"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="39"/>
       <c r="L46" s="6"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="35"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="36"/>
       <c r="L47" s="6"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="35"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="36"/>
       <c r="L48" s="6"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="35"/>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="36"/>
       <c r="L49" s="6"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="35"/>
+    <row r="50" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36"/>
       <c r="L50" s="6"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="14"/>
+    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="31"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="36"/>
       <c r="L51" s="6"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:16">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="14"/>
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="36"/>
       <c r="L52" s="6"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:16" ht="37.5" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" s="19">
-        <v>2</v>
-      </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="14"/>
+    <row r="53" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="36"/>
       <c r="L53" s="6"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:16">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="19">
-        <v>4</v>
-      </c>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="14"/>
+    <row r="54" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="36"/>
       <c r="L54" s="6"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:16">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="19">
-        <v>4</v>
-      </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="14"/>
+    <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="33"/>
       <c r="L55" s="6"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" s="19">
-        <v>3</v>
-      </c>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="14"/>
+    <row r="56" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="33"/>
       <c r="L56" s="6"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="19">
-        <v>5</v>
-      </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="14"/>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="33"/>
       <c r="L57" s="6"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="19">
-        <v>5</v>
-      </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="14"/>
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="33"/>
       <c r="L58" s="6"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:16">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" s="20">
-        <v>4</v>
-      </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
+    <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="33"/>
       <c r="L59" s="6"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:16">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="20">
-        <v>2</v>
-      </c>
-      <c r="G60" s="16"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="14"/>
       <c r="L60" s="6"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:16">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="27"/>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="G61" s="16"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="14"/>
       <c r="L61" s="6"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="1:16">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="27"/>
+    <row r="62" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="19">
+        <v>2</v>
+      </c>
       <c r="G62" s="16"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="14"/>
       <c r="L62" s="6"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:16">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="27"/>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="19">
+        <v>4</v>
+      </c>
       <c r="G63" s="16"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="14"/>
       <c r="L63" s="6"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:16">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="27"/>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="19">
+        <v>4</v>
+      </c>
       <c r="G64" s="16"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="14"/>
       <c r="L64" s="6"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="29">
-        <v>5</v>
-      </c>
-      <c r="O64" s="30"/>
-      <c r="P64" s="30"/>
-    </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="27"/>
+    </row>
+    <row r="65" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="19">
+        <v>3</v>
+      </c>
       <c r="G65" s="16"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="14"/>
       <c r="L65" s="6"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="29">
-        <v>4</v>
-      </c>
-      <c r="O65" s="30"/>
-      <c r="P65" s="30"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="27"/>
+    </row>
+    <row r="66" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="19">
+        <v>5</v>
+      </c>
       <c r="G66" s="16"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="14"/>
       <c r="L66" s="6"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="29">
-        <v>3</v>
-      </c>
-      <c r="O66" s="30"/>
-      <c r="P66" s="30"/>
-    </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="27"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="19">
+        <v>5</v>
+      </c>
       <c r="G67" s="16"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="14"/>
       <c r="L67" s="6"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="29">
-        <v>2</v>
-      </c>
-      <c r="O67" s="30"/>
-      <c r="P67" s="30"/>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="27"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="20">
+        <v>4</v>
+      </c>
       <c r="G68" s="16"/>
       <c r="H68" s="5"/>
       <c r="I68" s="6"/>
@@ -3863,19 +4252,18 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="2"/>
-      <c r="N68" s="29">
-        <v>1</v>
-      </c>
-      <c r="O68" s="30"/>
-      <c r="P68" s="30"/>
-    </row>
-    <row r="69" spans="1:16">
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="27"/>
+      <c r="E69" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" s="20">
+        <v>2</v>
+      </c>
       <c r="G69" s="16"/>
       <c r="H69" s="5"/>
       <c r="I69" s="6"/>
@@ -3883,19 +4271,18 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="29">
-        <v>0</v>
-      </c>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-    </row>
-    <row r="70" spans="1:16">
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="27"/>
+      <c r="E70" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" s="20">
+        <v>3</v>
+      </c>
       <c r="G70" s="16"/>
       <c r="H70" s="5"/>
       <c r="I70" s="6"/>
@@ -3903,13 +4290,8 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="2"/>
-      <c r="N70" s="29"/>
-      <c r="O70" s="30">
-        <v>2</v>
-      </c>
-      <c r="P70" s="30"/>
-    </row>
-    <row r="71" spans="1:16">
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -3923,13 +4305,8 @@
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="M71" s="2"/>
-      <c r="N71" s="29"/>
-      <c r="O71" s="30"/>
-      <c r="P71" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -3944,7 +4321,7 @@
       <c r="L72" s="6"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -3959,7 +4336,7 @@
       <c r="L73" s="6"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -3973,8 +4350,13 @@
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
       <c r="M74" s="2"/>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="N74" s="29">
+        <v>5</v>
+      </c>
+      <c r="O74" s="30"/>
+      <c r="P74" s="30"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -3988,8 +4370,13 @@
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="2"/>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="N75" s="29">
+        <v>4</v>
+      </c>
+      <c r="O75" s="30"/>
+      <c r="P75" s="30"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -4003,13 +4390,16 @@
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
       <c r="M76" s="2"/>
-    </row>
-    <row r="77" spans="1:16" ht="15.75" thickBot="1">
+      <c r="N76" s="29">
+        <v>3</v>
+      </c>
+      <c r="O76" s="30"/>
+      <c r="P76" s="30"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
-      <c r="B77" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C77" s="28"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="26"/>
       <c r="F77" s="27"/>
@@ -4020,38 +4410,53 @@
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
       <c r="M77" s="2"/>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="N77" s="29">
+        <v>2</v>
+      </c>
+      <c r="O77" s="30"/>
+      <c r="P77" s="30"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="98"/>
-      <c r="C78" s="99"/>
-      <c r="D78" s="99"/>
-      <c r="E78" s="99"/>
-      <c r="F78" s="99"/>
-      <c r="G78" s="99"/>
-      <c r="H78" s="99"/>
-      <c r="I78" s="99"/>
-      <c r="J78" s="100"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
       <c r="M78" s="2"/>
-    </row>
-    <row r="79" spans="1:16" ht="15.75" thickBot="1">
+      <c r="N78" s="29">
+        <v>1</v>
+      </c>
+      <c r="O78" s="30"/>
+      <c r="P78" s="30"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="101"/>
-      <c r="C79" s="102"/>
-      <c r="D79" s="102"/>
-      <c r="E79" s="102"/>
-      <c r="F79" s="102"/>
-      <c r="G79" s="102"/>
-      <c r="H79" s="102"/>
-      <c r="I79" s="102"/>
-      <c r="J79" s="103"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
       <c r="M79" s="2"/>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="N79" s="29">
+        <v>0</v>
+      </c>
+      <c r="O79" s="30"/>
+      <c r="P79" s="30"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -4065,258 +4470,437 @@
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
       <c r="M80" s="2"/>
-    </row>
-    <row r="81" spans="1:12" ht="15.75">
-      <c r="A81" s="93" t="s">
+      <c r="N80" s="29"/>
+      <c r="O80" s="30">
+        <v>2</v>
+      </c>
+      <c r="P80" s="30"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="29"/>
+      <c r="O81" s="30"/>
+      <c r="P81" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="2"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="28"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="2"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="7"/>
+      <c r="B88" s="102"/>
+      <c r="C88" s="103"/>
+      <c r="D88" s="103"/>
+      <c r="E88" s="103"/>
+      <c r="F88" s="103"/>
+      <c r="G88" s="103"/>
+      <c r="H88" s="103"/>
+      <c r="I88" s="103"/>
+      <c r="J88" s="104"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="105"/>
+      <c r="C89" s="106"/>
+      <c r="D89" s="106"/>
+      <c r="E89" s="106"/>
+      <c r="F89" s="106"/>
+      <c r="G89" s="106"/>
+      <c r="H89" s="106"/>
+      <c r="I89" s="106"/>
+      <c r="J89" s="107"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="2"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="7"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="34"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="2"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="2"/>
+    </row>
+    <row r="92" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="93"/>
-      <c r="C81" s="93"/>
-      <c r="D81" s="93"/>
-      <c r="E81" s="93"/>
-      <c r="F81" s="93"/>
-      <c r="G81" s="93"/>
-      <c r="H81" s="93"/>
-      <c r="I81" s="93"/>
-      <c r="J81" s="93"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-    </row>
-    <row r="82" spans="1:12">
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-    </row>
-    <row r="83" spans="1:12">
-      <c r="B83" s="73" t="s">
+      <c r="B92" s="97"/>
+      <c r="C92" s="97"/>
+      <c r="D92" s="97"/>
+      <c r="E92" s="97"/>
+      <c r="F92" s="97"/>
+      <c r="G92" s="97"/>
+      <c r="H92" s="97"/>
+      <c r="I92" s="97"/>
+      <c r="J92" s="97"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B94" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94" s="78"/>
+      <c r="D94" s="68">
+        <v>2</v>
+      </c>
+      <c r="E94" s="68"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="63"/>
+      <c r="I94" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="J94" s="63"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B95" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="C95" s="78"/>
+      <c r="D95" s="68">
+        <v>3</v>
+      </c>
+      <c r="E95" s="68"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H95" s="65"/>
+      <c r="I95" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="J95" s="99"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="74"/>
-      <c r="D83" s="64">
-        <v>2</v>
-      </c>
-      <c r="E83" s="64"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="H83" s="59"/>
-      <c r="I83" s="58" t="s">
+      <c r="C96" s="78"/>
+      <c r="D96" s="68"/>
+      <c r="E96" s="68"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J83" s="59"/>
-    </row>
-    <row r="84" spans="1:12">
-      <c r="B84" s="73" t="s">
+      <c r="H96" s="65"/>
+      <c r="I96" s="100" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96" s="101"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="74"/>
-      <c r="D84" s="64">
-        <v>3</v>
-      </c>
-      <c r="E84" s="64"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="60" t="s">
+      <c r="C97" s="78"/>
+      <c r="D97" s="68"/>
+      <c r="E97" s="68"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="H84" s="61"/>
-      <c r="I84" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="J84" s="95"/>
-    </row>
-    <row r="85" spans="1:12">
-      <c r="B85" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="74"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="60" t="s">
+      <c r="H97" s="65"/>
+      <c r="I97" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="J97" s="70"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G98" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="H85" s="61"/>
-      <c r="I85" s="96" t="s">
-        <v>21</v>
-      </c>
-      <c r="J85" s="97"/>
-    </row>
-    <row r="86" spans="1:12">
-      <c r="B86" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="74"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="60" t="s">
+      <c r="H98" s="67"/>
+      <c r="I98" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="J98" s="72"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G99" s="66">
+        <v>5</v>
+      </c>
+      <c r="H99" s="67"/>
+      <c r="I99" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H86" s="61"/>
-      <c r="I86" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="J86" s="66"/>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="G87" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="63"/>
-      <c r="I87" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="J87" s="68"/>
-    </row>
-    <row r="88" spans="1:12">
-      <c r="G88" s="62">
-        <v>5</v>
-      </c>
-      <c r="H88" s="63"/>
-      <c r="I88" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J88" s="57"/>
-    </row>
-    <row r="92" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A92" s="3"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="69"/>
-      <c r="I92" s="69"/>
-      <c r="J92" s="69"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="3"/>
-      <c r="B93" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="I93" s="70"/>
-      <c r="J93" s="70"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="23"/>
-    </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
-    </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-    </row>
-    <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="55"/>
-      <c r="E99" s="55"/>
-      <c r="F99" s="55"/>
-      <c r="G99" s="55"/>
-      <c r="H99" s="55"/>
-      <c r="I99" s="55"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
+      <c r="J99" s="61"/>
+    </row>
+    <row r="103" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="73"/>
+      <c r="J103" s="73"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" s="74"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="I104" s="74"/>
+      <c r="J104" s="74"/>
+      <c r="K104" s="23"/>
+      <c r="L104" s="23"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+    </row>
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="59"/>
+      <c r="F110" s="59"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="59"/>
+      <c r="I110" s="59"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="59">
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B78:J79"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="62">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A92:J92"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G4:H4"/>
@@ -4330,28 +4914,38 @@
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I86:J86"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="H103:J103"/>
+    <mergeCell ref="H104:J104"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B88:J89"/>
+    <mergeCell ref="B51:E54"/>
+    <mergeCell ref="A43:E46"/>
+    <mergeCell ref="A47:E50"/>
+    <mergeCell ref="F43:J46"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="I99:J99"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="F51:J54"/>
+    <mergeCell ref="K51:K54"/>
     <mergeCell ref="K43:K46"/>
     <mergeCell ref="F47:J50"/>
     <mergeCell ref="K47:K50"/>
-    <mergeCell ref="A43:E46"/>
-    <mergeCell ref="A47:E50"/>
-    <mergeCell ref="F43:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Reporte ED Acepte 5 Puntualizaciones CSS a Vista Principal
</commit_message>
<xml_diff>
--- a/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
+++ b/protected/modules/excel/templates/EvaluaciondeDesempenoTemplate.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teto\Desktop\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>Módulo de Evaluación de Desempeño</t>
   </si>
@@ -45,134 +50,140 @@
     <t>Resultados</t>
   </si>
   <si>
+    <t>EVALUACIÓN FINAL</t>
+  </si>
+  <si>
+    <t>RANGO</t>
+  </si>
+  <si>
+    <t>Rango</t>
+  </si>
+  <si>
+    <t>Interpretación</t>
+  </si>
+  <si>
+    <t>De 0 a 2</t>
+  </si>
+  <si>
+    <t>Más de 2 menos de 3</t>
+  </si>
+  <si>
+    <t>De 3 a menos de 4</t>
+  </si>
+  <si>
+    <t>De 4 a menos de 5</t>
+  </si>
+  <si>
+    <t>Desempeño Superior</t>
+  </si>
+  <si>
+    <t>Desempeño Sobresaliente</t>
+  </si>
+  <si>
+    <t>Desempeño Esperado</t>
+  </si>
+  <si>
+    <t>Oportunidad de Mejora</t>
+  </si>
+  <si>
+    <t>Desempeño Insuficiente</t>
+  </si>
+  <si>
+    <t>solucion</t>
+  </si>
+  <si>
+    <t>negociacion</t>
+  </si>
+  <si>
+    <t>planificacion</t>
+  </si>
+  <si>
+    <t>trabajar bajo presion</t>
+  </si>
+  <si>
+    <t>tomar decisiones</t>
+  </si>
+  <si>
+    <t>admnistrar tiempo</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>ade</t>
+  </si>
+  <si>
+    <t>Indicador</t>
+  </si>
+  <si>
+    <t>Compromiso</t>
+  </si>
+  <si>
+    <t>Puntaje</t>
+  </si>
+  <si>
+    <t>Cumpliendo con el plan estratégico de la Universidad, aplica los procedimientos que corresponden a la ejecución de las pruebas y todo lo que conlleva (coordinación de matrícula, coordinación de aulas, oidores, jurados, entre otros) interactúa con los clientes internos (compañeros de trabajo) y externos (estudiantes, Jurados y oidores), velar por la correcta aplicación de la Ordenanza y las buenas relaciones con las Sedes, con el fin de planificar y ejecutar el calendario Universitario de las Pruebas de Grado y toda la logística en tiempo establecido.</t>
+  </si>
+  <si>
+    <t>Competencia</t>
+  </si>
+  <si>
+    <t>investigacion</t>
+  </si>
+  <si>
+    <t>logro</t>
+  </si>
+  <si>
+    <t>orientacion</t>
+  </si>
+  <si>
+    <t>esfuerzo</t>
+  </si>
+  <si>
+    <t>Firma Evaluador</t>
+  </si>
+  <si>
+    <t>Firma Colaborador</t>
+  </si>
+  <si>
+    <t>Alineamiento organizacional</t>
+  </si>
+  <si>
+    <t>Pensamiento estrategico</t>
+  </si>
+  <si>
+    <t>Toma de decisiones</t>
+  </si>
+  <si>
+    <t>Fecha de Registro de Evaluación:</t>
+  </si>
+  <si>
+    <t>Fecha de Registro de Compromisos:</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Escala</t>
+  </si>
+  <si>
     <t>Nivel Puntualizaciones</t>
   </si>
   <si>
     <t>Nivel Competencias</t>
   </si>
   <si>
-    <t>EVALUACIÓN FINAL</t>
-  </si>
-  <si>
-    <t>RANGO</t>
-  </si>
-  <si>
-    <t>Rango</t>
-  </si>
-  <si>
-    <t>Interpretación</t>
-  </si>
-  <si>
-    <t>De 0 a 2</t>
-  </si>
-  <si>
-    <t>Más de 2 menos de 3</t>
-  </si>
-  <si>
-    <t>De 3 a menos de 4</t>
-  </si>
-  <si>
-    <t>De 4 a menos de 5</t>
-  </si>
-  <si>
-    <t>Desempeño Superior</t>
-  </si>
-  <si>
-    <t>Desempeño Sobresaliente</t>
-  </si>
-  <si>
-    <t>Desempeño Esperado</t>
-  </si>
-  <si>
-    <t>Oportunidad de Mejora</t>
-  </si>
-  <si>
-    <t>Desempeño Insuficiente</t>
-  </si>
-  <si>
-    <t>solucion</t>
-  </si>
-  <si>
-    <t>negociacion</t>
-  </si>
-  <si>
-    <t>planificacion</t>
-  </si>
-  <si>
-    <t>trabajar bajo presion</t>
-  </si>
-  <si>
-    <t>tomar decisiones</t>
-  </si>
-  <si>
-    <t>admnistrar tiempo</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>ade</t>
-  </si>
-  <si>
-    <t>Indicador</t>
-  </si>
-  <si>
-    <t>Compromiso</t>
-  </si>
-  <si>
-    <t>Puntaje</t>
-  </si>
-  <si>
-    <t>Cumpliendo con el plan estratégico de la Universidad, aplica los procedimientos que corresponden a la ejecución de las pruebas y todo lo que conlleva (coordinación de matrícula, coordinación de aulas, oidores, jurados, entre otros) interactúa con los clientes internos (compañeros de trabajo) y externos (estudiantes, Jurados y oidores), velar por la correcta aplicación de la Ordenanza y las buenas relaciones con las Sedes, con el fin de planificar y ejecutar el calendario Universitario de las Pruebas de Grado y toda la logística en tiempo establecido.</t>
-  </si>
-  <si>
-    <t>Competencia</t>
-  </si>
-  <si>
-    <t>investigacion</t>
-  </si>
-  <si>
-    <t>logro</t>
-  </si>
-  <si>
-    <t>orientacion</t>
-  </si>
-  <si>
-    <t>esfuerzo</t>
-  </si>
-  <si>
-    <t>kkel</t>
-  </si>
-  <si>
-    <t>Firma Evaluador</t>
-  </si>
-  <si>
-    <t>Firma Colaborador</t>
-  </si>
-  <si>
-    <t>Alineamiento organizacional</t>
-  </si>
-  <si>
-    <t>Pensamiento estrategico</t>
-  </si>
-  <si>
-    <t>Toma de decisiones</t>
-  </si>
-  <si>
-    <t>Fecha de Registro de Evaluación:</t>
-  </si>
-  <si>
-    <t>Fecha de Registro de Compromisos:</t>
-  </si>
-  <si>
-    <t>Comentarios</t>
+    <t>trabajo</t>
+  </si>
+  <si>
+    <t>equipo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -633,6 +644,28 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -645,13 +678,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
@@ -853,27 +879,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -895,7 +921,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -929,6 +965,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -937,6 +974,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -946,6 +984,7 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -973,6 +1012,7 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -997,6 +1037,7 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1021,6 +1062,7 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1045,6 +1087,7 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1069,6 +1112,7 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1093,6 +1137,7 @@
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1117,6 +1162,7 @@
         <c:ser>
           <c:idx val="7"/>
           <c:order val="7"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1141,6 +1187,7 @@
         <c:ser>
           <c:idx val="8"/>
           <c:order val="8"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1165,6 +1212,7 @@
         <c:ser>
           <c:idx val="9"/>
           <c:order val="9"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1189,6 +1237,7 @@
         <c:ser>
           <c:idx val="10"/>
           <c:order val="10"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1213,6 +1262,7 @@
         <c:ser>
           <c:idx val="11"/>
           <c:order val="11"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1237,6 +1287,7 @@
         <c:ser>
           <c:idx val="12"/>
           <c:order val="12"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1261,6 +1312,7 @@
         <c:ser>
           <c:idx val="13"/>
           <c:order val="13"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1285,6 +1337,7 @@
         <c:ser>
           <c:idx val="14"/>
           <c:order val="14"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1309,6 +1362,7 @@
         <c:ser>
           <c:idx val="15"/>
           <c:order val="15"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$K$34</c:f>
@@ -1330,13 +1384,121 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$K$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Puntaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="91136384"/>
-        <c:axId val="91137920"/>
+        <c:axId val="182558584"/>
+        <c:axId val="182558976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91136384"/>
+        <c:axId val="182558584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,18 +1506,21 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="91137920"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="182558976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91137920"/>
+        <c:axId val="182558976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1398,6 +1563,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1408,6 +1574,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1433,10 +1600,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91136384"/>
+        <c:crossAx val="182558584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1450,6 +1617,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1473,12 +1641,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1486,7 +1654,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1520,6 +1698,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1528,6 +1707,7 @@
         <a:effectLst/>
       </c:spPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1539,7 +1719,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$52</c:f>
+              <c:f>Sheet1!$F$61</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1548,11 +1728,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$E$53:$E$60</c:f>
+              <c:f>Sheet1!$E$62:$E$70</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Alineamiento organizacional</c:v>
                 </c:pt>
@@ -1575,17 +1756,20 @@
                   <c:v>esfuerzo</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>kkel</c:v>
+                  <c:v>trabajo</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>equipo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$53:$F$60</c:f>
+              <c:f>Sheet1!$F$62:$F$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1609,18 +1793,29 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="91957504"/>
-        <c:axId val="91971584"/>
+        <c:axId val="182559760"/>
+        <c:axId val="182560152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91957504"/>
+        <c:axId val="182559760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1628,18 +1823,21 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="91971584"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="182560152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91971584"/>
+        <c:axId val="182560152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1682,6 +1880,7 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1692,6 +1891,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1717,10 +1917,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91957504"/>
+        <c:crossAx val="182559760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1734,6 +1934,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1757,12 +1958,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1770,7 +1971,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="es-ES"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1799,6 +2010,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1806,12 +2018,34 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CR"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1826,9 +2060,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$64</c:f>
+              <c:f>Sheet1!$N$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1851,9 +2103,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$65</c:f>
+              <c:f>Sheet1!$N$75</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1876,9 +2146,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$66</c:f>
+              <c:f>Sheet1!$N$76</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1901,9 +2189,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$67</c:f>
+              <c:f>Sheet1!$N$77</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1926,9 +2232,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$68</c:f>
+              <c:f>Sheet1!$N$78</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1951,9 +2275,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$69</c:f>
+              <c:f>Sheet1!$N$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1976,16 +2318,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:delete val="1"/>
-            </c:dLbl>
-            <c:showVal val="1"/>
-          </c:dLbls>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$70:$P$70</c:f>
+              <c:f>Sheet1!$N$80:$P$80</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2010,9 +2363,27 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$82:$P$82</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Escala</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Nivel Puntualizaciones</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Nivel Competencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$71:$P$71</c:f>
+              <c:f>Sheet1!$N$81:$P$81</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2023,32 +2394,28 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="93406336"/>
-        <c:axId val="93407872"/>
+        <c:axId val="183498408"/>
+        <c:axId val="183498800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93406336"/>
+        <c:axId val="183498408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:tickLblPos val="none"/>
-        <c:crossAx val="93407872"/>
-        <c:crosses val="autoZero"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="93407872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -2074,10 +2441,55 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93406336"/>
+        <c:crossAx val="183498800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="183498800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="183498408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2091,6 +2503,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2114,12 +2527,12 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2729,13 +3142,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>1114425</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2801,7 +3214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2836,7 +3249,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3013,22 +3426,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94:E94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
@@ -3045,207 +3458,207 @@
     <col min="13" max="13" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="76" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
       <c r="L2" s="9"/>
     </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="71" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="71"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="71" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="30" customHeight="1">
-      <c r="B6" s="90" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="94"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="72"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
+      <c r="G6" s="76" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
-      <c r="A9" s="93" t="s">
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K11" s="10"/>
       <c r="L11" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K12" s="10"/>
       <c r="L12" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K13" s="10"/>
       <c r="L13" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K14" s="10"/>
       <c r="L14" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K17" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L17" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L18" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L19" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L20" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K21" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L21" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L22" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L23" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L24" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -3259,7 +3672,7 @@
       <c r="L32" s="6"/>
       <c r="M32" s="2"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -3273,589 +3686,565 @@
       <c r="L33" s="6"/>
       <c r="M33" s="2"/>
     </row>
-    <row r="34" spans="1:13">
-      <c r="A34" s="77" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="81"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="81"/>
+      <c r="E34" s="81"/>
+      <c r="F34" s="81" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="21" t="s">
-        <v>33</v>
       </c>
       <c r="L34" s="6"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" ht="15" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="46"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="78">
+    <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="41"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="82">
         <v>2</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="2"/>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="39"/>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="79"/>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="83"/>
       <c r="L36" s="6"/>
       <c r="M36" s="2"/>
     </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="39"/>
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="51"/>
-      <c r="K37" s="79"/>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="43"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="83"/>
       <c r="L37" s="6"/>
       <c r="M37" s="2"/>
     </row>
-    <row r="38" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A38" s="42"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="44"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="80"/>
+    <row r="38" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="57"/>
+      <c r="I38" s="57"/>
+      <c r="J38" s="58"/>
+      <c r="K38" s="84"/>
       <c r="L38" s="6"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="81"/>
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="83"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="47"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="31"/>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="85"/>
+      <c r="B39" s="86"/>
+      <c r="C39" s="86"/>
+      <c r="D39" s="86"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="37"/>
       <c r="L39" s="6"/>
       <c r="M39" s="2"/>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="84"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="85"/>
-      <c r="D40" s="85"/>
-      <c r="E40" s="86"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="51"/>
-      <c r="K40" s="32"/>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="88"/>
+      <c r="B40" s="89"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="89"/>
+      <c r="E40" s="90"/>
+      <c r="F40" s="53"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="38"/>
       <c r="L40" s="6"/>
       <c r="M40" s="2"/>
     </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="84"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="85"/>
-      <c r="D41" s="85"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="50"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="51"/>
-      <c r="K41" s="32"/>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="88"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="89"/>
+      <c r="D41" s="89"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="53"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="38"/>
       <c r="L41" s="6"/>
       <c r="M41" s="2"/>
     </row>
-    <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A42" s="87"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="88"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="89"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="33"/>
+    <row r="42" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="91"/>
+      <c r="B42" s="92"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="58"/>
+      <c r="K42" s="39"/>
       <c r="L42" s="6"/>
       <c r="M42" s="2"/>
     </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="36"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
-      <c r="I43" s="47"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="31"/>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="40"/>
+      <c r="B43" s="41"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="37"/>
       <c r="L43" s="6"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="32"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="43"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="53"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="38"/>
       <c r="L44" s="6"/>
       <c r="M44" s="2"/>
     </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="39"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="32"/>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="43"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="53"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="38"/>
       <c r="L45" s="6"/>
       <c r="M45" s="2"/>
     </row>
-    <row r="46" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="53"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="33"/>
+    <row r="46" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="46"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="57"/>
+      <c r="I46" s="57"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="39"/>
       <c r="L46" s="6"/>
       <c r="M46" s="2"/>
     </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="45"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="34"/>
-      <c r="K47" s="35"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="49"/>
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="35"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="36"/>
       <c r="L47" s="6"/>
       <c r="M47" s="2"/>
     </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="34"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="34"/>
-      <c r="K48" s="35"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="36"/>
       <c r="L48" s="6"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="1:16">
-      <c r="A49" s="45"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
-      <c r="J49" s="34"/>
-      <c r="K49" s="35"/>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="36"/>
       <c r="L49" s="6"/>
       <c r="M49" s="2"/>
     </row>
-    <row r="50" spans="1:16" ht="26.25" customHeight="1">
-      <c r="A50" s="45"/>
-      <c r="B50" s="45"/>
-      <c r="C50" s="45"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="34"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="35"/>
+    <row r="50" spans="1:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="35"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="36"/>
       <c r="L50" s="6"/>
       <c r="M50" s="2"/>
     </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="K51" s="14"/>
+    <row r="51" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="31"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="35"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="36"/>
       <c r="L51" s="6"/>
       <c r="M51" s="2"/>
     </row>
-    <row r="52" spans="1:16">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="15"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="K52" s="14"/>
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="31"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="49"/>
+      <c r="D52" s="49"/>
+      <c r="E52" s="49"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="35"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="35"/>
+      <c r="K52" s="36"/>
       <c r="L52" s="6"/>
       <c r="M52" s="2"/>
     </row>
-    <row r="53" spans="1:16" ht="37.5" customHeight="1">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" s="19">
-        <v>2</v>
-      </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="K53" s="14"/>
+    <row r="53" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="31"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="49"/>
+      <c r="D53" s="49"/>
+      <c r="E53" s="49"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="35"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="35"/>
+      <c r="K53" s="36"/>
       <c r="L53" s="6"/>
       <c r="M53" s="2"/>
     </row>
-    <row r="54" spans="1:16">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F54" s="19">
-        <v>4</v>
-      </c>
-      <c r="G54" s="16"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="K54" s="14"/>
+    <row r="54" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="31"/>
+      <c r="B54" s="49"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="49"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="36"/>
       <c r="L54" s="6"/>
       <c r="M54" s="2"/>
     </row>
-    <row r="55" spans="1:16">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="19">
-        <v>4</v>
-      </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="K55" s="14"/>
+    <row r="55" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="31"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="33"/>
       <c r="L55" s="6"/>
       <c r="M55" s="2"/>
     </row>
-    <row r="56" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" s="19">
-        <v>3</v>
-      </c>
-      <c r="G56" s="16"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="14"/>
+    <row r="56" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="32"/>
+      <c r="J56" s="32"/>
+      <c r="K56" s="33"/>
       <c r="L56" s="6"/>
       <c r="M56" s="2"/>
     </row>
-    <row r="57" spans="1:16" ht="16.5" customHeight="1">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="19">
-        <v>5</v>
-      </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="K57" s="14"/>
+    <row r="57" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31"/>
+      <c r="B57" s="31"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="32"/>
+      <c r="K57" s="33"/>
       <c r="L57" s="6"/>
       <c r="M57" s="2"/>
     </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F58" s="19">
-        <v>5</v>
-      </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
-      <c r="K58" s="14"/>
+    <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="32"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="33"/>
       <c r="L58" s="6"/>
       <c r="M58" s="2"/>
     </row>
-    <row r="59" spans="1:16">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" s="20">
-        <v>4</v>
-      </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
+    <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31"/>
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="33"/>
       <c r="L59" s="6"/>
       <c r="M59" s="2"/>
     </row>
-    <row r="60" spans="1:16">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F60" s="20">
-        <v>2</v>
-      </c>
-      <c r="G60" s="16"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="14"/>
       <c r="L60" s="6"/>
       <c r="M60" s="2"/>
     </row>
-    <row r="61" spans="1:16">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="27"/>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F61" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="G61" s="16"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="6"/>
-      <c r="K61" s="6"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="14"/>
       <c r="L61" s="6"/>
       <c r="M61" s="2"/>
     </row>
-    <row r="62" spans="1:16">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="27"/>
+    <row r="62" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="19">
+        <v>2</v>
+      </c>
       <c r="G62" s="16"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="6"/>
-      <c r="K62" s="6"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="14"/>
       <c r="L62" s="6"/>
       <c r="M62" s="2"/>
     </row>
-    <row r="63" spans="1:16">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="27"/>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F63" s="19">
+        <v>4</v>
+      </c>
       <c r="G63" s="16"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="14"/>
       <c r="L63" s="6"/>
       <c r="M63" s="2"/>
     </row>
-    <row r="64" spans="1:16">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="27"/>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" s="19">
+        <v>4</v>
+      </c>
       <c r="G64" s="16"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="6"/>
-      <c r="K64" s="6"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="14"/>
       <c r="L64" s="6"/>
       <c r="M64" s="2"/>
-      <c r="N64" s="29">
-        <v>5</v>
-      </c>
-      <c r="O64" s="30"/>
-      <c r="P64" s="30"/>
-    </row>
-    <row r="65" spans="1:16">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="27"/>
+    </row>
+    <row r="65" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F65" s="19">
+        <v>3</v>
+      </c>
       <c r="G65" s="16"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="6"/>
-      <c r="K65" s="6"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="14"/>
       <c r="L65" s="6"/>
       <c r="M65" s="2"/>
-      <c r="N65" s="29">
-        <v>4</v>
-      </c>
-      <c r="O65" s="30"/>
-      <c r="P65" s="30"/>
-    </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="27"/>
+    </row>
+    <row r="66" spans="1:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="19">
+        <v>5</v>
+      </c>
       <c r="G66" s="16"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="6"/>
-      <c r="J66" s="6"/>
-      <c r="K66" s="6"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="14"/>
       <c r="L66" s="6"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="29">
-        <v>3</v>
-      </c>
-      <c r="O66" s="30"/>
-      <c r="P66" s="30"/>
-    </row>
-    <row r="67" spans="1:16">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="27"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="19">
+        <v>5</v>
+      </c>
       <c r="G67" s="16"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="14"/>
       <c r="L67" s="6"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="29">
-        <v>2</v>
-      </c>
-      <c r="O67" s="30"/>
-      <c r="P67" s="30"/>
-    </row>
-    <row r="68" spans="1:16">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="27"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="20">
+        <v>4</v>
+      </c>
       <c r="G68" s="16"/>
       <c r="H68" s="5"/>
       <c r="I68" s="6"/>
@@ -3863,19 +4252,18 @@
       <c r="K68" s="6"/>
       <c r="L68" s="6"/>
       <c r="M68" s="2"/>
-      <c r="N68" s="29">
-        <v>1</v>
-      </c>
-      <c r="O68" s="30"/>
-      <c r="P68" s="30"/>
-    </row>
-    <row r="69" spans="1:16">
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="27"/>
+      <c r="E69" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F69" s="20">
+        <v>2</v>
+      </c>
       <c r="G69" s="16"/>
       <c r="H69" s="5"/>
       <c r="I69" s="6"/>
@@ -3883,19 +4271,18 @@
       <c r="K69" s="6"/>
       <c r="L69" s="6"/>
       <c r="M69" s="2"/>
-      <c r="N69" s="29">
-        <v>0</v>
-      </c>
-      <c r="O69" s="30"/>
-      <c r="P69" s="30"/>
-    </row>
-    <row r="70" spans="1:16">
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="27"/>
+      <c r="E70" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" s="20">
+        <v>3</v>
+      </c>
       <c r="G70" s="16"/>
       <c r="H70" s="5"/>
       <c r="I70" s="6"/>
@@ -3903,13 +4290,8 @@
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
       <c r="M70" s="2"/>
-      <c r="N70" s="29"/>
-      <c r="O70" s="30">
-        <v>2</v>
-      </c>
-      <c r="P70" s="30"/>
-    </row>
-    <row r="71" spans="1:16">
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -3923,13 +4305,8 @@
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="M71" s="2"/>
-      <c r="N71" s="29"/>
-      <c r="O71" s="30"/>
-      <c r="P71" s="30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -3944,7 +4321,7 @@
       <c r="L72" s="6"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -3959,7 +4336,7 @@
       <c r="L73" s="6"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -3973,8 +4350,13 @@
       <c r="K74" s="6"/>
       <c r="L74" s="6"/>
       <c r="M74" s="2"/>
-    </row>
-    <row r="75" spans="1:16">
+      <c r="N74" s="29">
+        <v>5</v>
+      </c>
+      <c r="O74" s="30"/>
+      <c r="P74" s="30"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -3988,8 +4370,13 @@
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="M75" s="2"/>
-    </row>
-    <row r="76" spans="1:16">
+      <c r="N75" s="29">
+        <v>4</v>
+      </c>
+      <c r="O75" s="30"/>
+      <c r="P75" s="30"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -4003,13 +4390,16 @@
       <c r="K76" s="6"/>
       <c r="L76" s="6"/>
       <c r="M76" s="2"/>
-    </row>
-    <row r="77" spans="1:16" ht="15.75" thickBot="1">
+      <c r="N76" s="29">
+        <v>3</v>
+      </c>
+      <c r="O76" s="30"/>
+      <c r="P76" s="30"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="7"/>
-      <c r="B77" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C77" s="28"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="26"/>
       <c r="F77" s="27"/>
@@ -4020,38 +4410,53 @@
       <c r="K77" s="6"/>
       <c r="L77" s="6"/>
       <c r="M77" s="2"/>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="N77" s="29">
+        <v>2</v>
+      </c>
+      <c r="O77" s="30"/>
+      <c r="P77" s="30"/>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="7"/>
-      <c r="B78" s="98"/>
-      <c r="C78" s="99"/>
-      <c r="D78" s="99"/>
-      <c r="E78" s="99"/>
-      <c r="F78" s="99"/>
-      <c r="G78" s="99"/>
-      <c r="H78" s="99"/>
-      <c r="I78" s="99"/>
-      <c r="J78" s="100"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="26"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
       <c r="M78" s="2"/>
-    </row>
-    <row r="79" spans="1:16" ht="15.75" thickBot="1">
+      <c r="N78" s="29">
+        <v>1</v>
+      </c>
+      <c r="O78" s="30"/>
+      <c r="P78" s="30"/>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="7"/>
-      <c r="B79" s="101"/>
-      <c r="C79" s="102"/>
-      <c r="D79" s="102"/>
-      <c r="E79" s="102"/>
-      <c r="F79" s="102"/>
-      <c r="G79" s="102"/>
-      <c r="H79" s="102"/>
-      <c r="I79" s="102"/>
-      <c r="J79" s="103"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="26"/>
+      <c r="F79" s="27"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
       <c r="K79" s="6"/>
       <c r="L79" s="6"/>
       <c r="M79" s="2"/>
-    </row>
-    <row r="80" spans="1:16">
+      <c r="N79" s="29">
+        <v>0</v>
+      </c>
+      <c r="O79" s="30"/>
+      <c r="P79" s="30"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -4065,258 +4470,437 @@
       <c r="K80" s="6"/>
       <c r="L80" s="6"/>
       <c r="M80" s="2"/>
-    </row>
-    <row r="81" spans="1:12" ht="15.75">
-      <c r="A81" s="93" t="s">
+      <c r="N80" s="29"/>
+      <c r="O80" s="30">
+        <v>2</v>
+      </c>
+      <c r="P80" s="30"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="27"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="29"/>
+      <c r="O81" s="30"/>
+      <c r="P81" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="27"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O82" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="P82" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="26"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="2"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="27"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="2"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="27"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="2"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="27"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="2"/>
+    </row>
+    <row r="87" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7"/>
+      <c r="B87" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="28"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="2"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="7"/>
+      <c r="B88" s="102"/>
+      <c r="C88" s="103"/>
+      <c r="D88" s="103"/>
+      <c r="E88" s="103"/>
+      <c r="F88" s="103"/>
+      <c r="G88" s="103"/>
+      <c r="H88" s="103"/>
+      <c r="I88" s="103"/>
+      <c r="J88" s="104"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="2"/>
+    </row>
+    <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7"/>
+      <c r="B89" s="105"/>
+      <c r="C89" s="106"/>
+      <c r="D89" s="106"/>
+      <c r="E89" s="106"/>
+      <c r="F89" s="106"/>
+      <c r="G89" s="106"/>
+      <c r="H89" s="106"/>
+      <c r="I89" s="106"/>
+      <c r="J89" s="107"/>
+      <c r="K89" s="6"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="2"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="7"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="34"/>
+      <c r="K90" s="6"/>
+      <c r="L90" s="6"/>
+      <c r="M90" s="2"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="26"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="2"/>
+    </row>
+    <row r="92" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A92" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="93"/>
-      <c r="C81" s="93"/>
-      <c r="D81" s="93"/>
-      <c r="E81" s="93"/>
-      <c r="F81" s="93"/>
-      <c r="G81" s="93"/>
-      <c r="H81" s="93"/>
-      <c r="I81" s="93"/>
-      <c r="J81" s="93"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-    </row>
-    <row r="82" spans="1:12">
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-    </row>
-    <row r="83" spans="1:12">
-      <c r="B83" s="73" t="s">
+      <c r="B92" s="97"/>
+      <c r="C92" s="97"/>
+      <c r="D92" s="97"/>
+      <c r="E92" s="97"/>
+      <c r="F92" s="97"/>
+      <c r="G92" s="97"/>
+      <c r="H92" s="97"/>
+      <c r="I92" s="97"/>
+      <c r="J92" s="97"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="4"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B94" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C94" s="78"/>
+      <c r="D94" s="68">
+        <v>2</v>
+      </c>
+      <c r="E94" s="68"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="H94" s="63"/>
+      <c r="I94" s="62" t="s">
+        <v>11</v>
+      </c>
+      <c r="J94" s="63"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B95" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="C95" s="78"/>
+      <c r="D95" s="68">
+        <v>3</v>
+      </c>
+      <c r="E95" s="68"/>
+      <c r="F95" s="3"/>
+      <c r="G95" s="64" t="s">
+        <v>12</v>
+      </c>
+      <c r="H95" s="65"/>
+      <c r="I95" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="J95" s="99"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B96" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C83" s="74"/>
-      <c r="D83" s="64">
-        <v>2</v>
-      </c>
-      <c r="E83" s="64"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="H83" s="59"/>
-      <c r="I83" s="58" t="s">
+      <c r="C96" s="78"/>
+      <c r="D96" s="68"/>
+      <c r="E96" s="68"/>
+      <c r="F96" s="3"/>
+      <c r="G96" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="J83" s="59"/>
-    </row>
-    <row r="84" spans="1:12">
-      <c r="B84" s="73" t="s">
+      <c r="H96" s="65"/>
+      <c r="I96" s="100" t="s">
+        <v>19</v>
+      </c>
+      <c r="J96" s="101"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="C84" s="74"/>
-      <c r="D84" s="64">
-        <v>3</v>
-      </c>
-      <c r="E84" s="64"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="60" t="s">
+      <c r="C97" s="78"/>
+      <c r="D97" s="68"/>
+      <c r="E97" s="68"/>
+      <c r="F97" s="3"/>
+      <c r="G97" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="H84" s="61"/>
-      <c r="I84" s="94" t="s">
-        <v>22</v>
-      </c>
-      <c r="J84" s="95"/>
-    </row>
-    <row r="85" spans="1:12">
-      <c r="B85" s="73" t="s">
-        <v>10</v>
-      </c>
-      <c r="C85" s="74"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="60" t="s">
+      <c r="H97" s="65"/>
+      <c r="I97" s="69" t="s">
+        <v>18</v>
+      </c>
+      <c r="J97" s="70"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G98" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="H85" s="61"/>
-      <c r="I85" s="96" t="s">
-        <v>21</v>
-      </c>
-      <c r="J85" s="97"/>
-    </row>
-    <row r="86" spans="1:12">
-      <c r="B86" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="C86" s="74"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="60" t="s">
+      <c r="H98" s="67"/>
+      <c r="I98" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="J98" s="72"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G99" s="66">
+        <v>5</v>
+      </c>
+      <c r="H99" s="67"/>
+      <c r="I99" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H86" s="61"/>
-      <c r="I86" s="65" t="s">
-        <v>20</v>
-      </c>
-      <c r="J86" s="66"/>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="G87" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="63"/>
-      <c r="I87" s="67" t="s">
-        <v>19</v>
-      </c>
-      <c r="J87" s="68"/>
-    </row>
-    <row r="88" spans="1:12">
-      <c r="G88" s="62">
-        <v>5</v>
-      </c>
-      <c r="H88" s="63"/>
-      <c r="I88" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="J88" s="57"/>
-    </row>
-    <row r="92" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A92" s="3"/>
-      <c r="B92" s="22"/>
-      <c r="C92" s="22"/>
-      <c r="D92" s="22"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="69"/>
-      <c r="I92" s="69"/>
-      <c r="J92" s="69"/>
-      <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
-    </row>
-    <row r="93" spans="1:12">
-      <c r="A93" s="3"/>
-      <c r="B93" s="70" t="s">
-        <v>41</v>
-      </c>
-      <c r="C93" s="70"/>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70"/>
-      <c r="F93" s="23"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="I93" s="70"/>
-      <c r="J93" s="70"/>
-      <c r="K93" s="23"/>
-      <c r="L93" s="23"/>
-    </row>
-    <row r="94" spans="1:12">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
-    </row>
-    <row r="95" spans="1:12">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-    </row>
-    <row r="97" spans="1:10" ht="15.75">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
-      <c r="E97" s="4"/>
-      <c r="F97" s="4"/>
-      <c r="G97" s="4"/>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-      <c r="J97" s="4"/>
-    </row>
-    <row r="99" spans="1:10">
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="55"/>
-      <c r="E99" s="55"/>
-      <c r="F99" s="55"/>
-      <c r="G99" s="55"/>
-      <c r="H99" s="55"/>
-      <c r="I99" s="55"/>
-    </row>
-    <row r="100" spans="1:10">
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="1:10">
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:10">
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
+      <c r="J99" s="61"/>
+    </row>
+    <row r="103" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3"/>
+      <c r="B103" s="22"/>
+      <c r="C103" s="22"/>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="73"/>
+      <c r="I103" s="73"/>
+      <c r="J103" s="73"/>
+      <c r="K103" s="3"/>
+      <c r="L103" s="3"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+      <c r="B104" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C104" s="74"/>
+      <c r="D104" s="74"/>
+      <c r="E104" s="74"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="I104" s="74"/>
+      <c r="J104" s="74"/>
+      <c r="K104" s="23"/>
+      <c r="L104" s="23"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+      <c r="D105" s="3"/>
+      <c r="E105" s="3"/>
+      <c r="F105" s="3"/>
+      <c r="G105" s="3"/>
+      <c r="H105" s="3"/>
+      <c r="I105" s="3"/>
+      <c r="J105" s="3"/>
+      <c r="K105" s="3"/>
+      <c r="L105" s="3"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
+      <c r="E106" s="3"/>
+      <c r="F106" s="3"/>
+      <c r="G106" s="3"/>
+      <c r="H106" s="3"/>
+      <c r="I106" s="3"/>
+      <c r="J106" s="3"/>
+      <c r="K106" s="3"/>
+      <c r="L106" s="3"/>
+    </row>
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="4"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="4"/>
+      <c r="D108" s="4"/>
+      <c r="E108" s="4"/>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+      <c r="I108" s="4"/>
+      <c r="J108" s="4"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="59"/>
+      <c r="E110" s="59"/>
+      <c r="F110" s="59"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="59"/>
+      <c r="I110" s="59"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
+      <c r="E111" s="3"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="3"/>
+      <c r="I111" s="3"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="3"/>
+      <c r="I113" s="3"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="59">
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="I84:J84"/>
-    <mergeCell ref="I85:J85"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B78:J79"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="62">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A92:J92"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="I95:J95"/>
+    <mergeCell ref="I96:J96"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="G4:H4"/>
@@ -4330,28 +4914,38 @@
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="F99:G99"/>
-    <mergeCell ref="H99:I99"/>
-    <mergeCell ref="I88:J88"/>
-    <mergeCell ref="G83:H83"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="G85:H85"/>
-    <mergeCell ref="G86:H86"/>
-    <mergeCell ref="G87:H87"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="G88:H88"/>
-    <mergeCell ref="I86:J86"/>
-    <mergeCell ref="I87:J87"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I98:J98"/>
+    <mergeCell ref="H103:J103"/>
+    <mergeCell ref="H104:J104"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="B88:J89"/>
+    <mergeCell ref="B51:E54"/>
+    <mergeCell ref="A43:E46"/>
+    <mergeCell ref="A47:E50"/>
+    <mergeCell ref="F43:J46"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="F110:G110"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="I99:J99"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="I97:J97"/>
+    <mergeCell ref="F51:J54"/>
+    <mergeCell ref="K51:K54"/>
     <mergeCell ref="K43:K46"/>
     <mergeCell ref="F47:J50"/>
     <mergeCell ref="K47:K50"/>
-    <mergeCell ref="A43:E46"/>
-    <mergeCell ref="A47:E50"/>
-    <mergeCell ref="F43:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>